<commit_message>
subindo o projeto completo
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog-Projeto-Zelda.xlsx
+++ b/Documentação/Backlog/Backlog-Projeto-Zelda.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4637e3830c875062/Área de Trabalho/Projeto Zelda/TheLegendsofZelda/Documentação/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{BC7563BB-D0FE-4AA5-8B85-FA70BBD6FEB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2AE8C8BE-34D1-4499-91AC-83A63B4B9017}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{BC7563BB-D0FE-4AA5-8B85-FA70BBD6FEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F7E22D-7EA5-47F9-BBFE-4174E42E8A21}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20B32848-DFCA-478A-88E4-DFC2AB9FEDEF}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Requisito</t>
   </si>
@@ -54,18 +51,9 @@
     <t>Ordem de execução</t>
   </si>
   <si>
-    <t>Tela de login</t>
-  </si>
-  <si>
     <t>O usuário será verificado no banco de dados, e se ele estiver cadastrado, terá acesso ao sistema</t>
   </si>
   <si>
-    <t xml:space="preserve">importante </t>
-  </si>
-  <si>
-    <t>Tela de cadastro</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
@@ -75,21 +63,9 @@
     <t xml:space="preserve">Site institucional </t>
   </si>
   <si>
-    <t xml:space="preserve">Onde o usuário terá acesso as informações da empresa </t>
-  </si>
-  <si>
-    <t>essencial</t>
-  </si>
-  <si>
     <t>banco de dados</t>
   </si>
   <si>
-    <t>Planilha de risco</t>
-  </si>
-  <si>
-    <t>Funcional</t>
-  </si>
-  <si>
     <t>Coletar dados dos clientes interessados e rigistra-los no banco de dados</t>
   </si>
   <si>
@@ -99,33 +75,71 @@
     <t>Onde sera armazenado os dados dos clientes e os dados registrados pelo site</t>
   </si>
   <si>
-    <t>Planilha  detalhada com possiveis riscos</t>
-  </si>
-  <si>
     <t>Modelagem DER/MER das tabelas do banco de dados</t>
   </si>
   <si>
     <t>Modelagem logica de dados</t>
   </si>
   <si>
-    <t>Relatorio de projeto</t>
-  </si>
-  <si>
-    <t>Relatorio detalhado com informações relacionadas ao projeto</t>
-  </si>
-  <si>
-    <t>conecxão entre site, api e o banco de dados</t>
-  </si>
-  <si>
     <t>Para o armazenamento e consulta de dados entre o site e o banco.</t>
+  </si>
+  <si>
+    <t>modal de login</t>
+  </si>
+  <si>
+    <t>modal de cadastro</t>
+  </si>
+  <si>
+    <t>Onde o usuário terá acesso as informações do site</t>
+  </si>
+  <si>
+    <t>fórum de descussão</t>
+  </si>
+  <si>
+    <t>O usuário terá acesso a uma tela onde entrará em contato com outros usuários do site para discutir assuntos pertinentes ao tema</t>
+  </si>
+  <si>
+    <t>Edital</t>
+  </si>
+  <si>
+    <t>Local no site destinado á noticias publicadas por adiministradores da página aos usuários</t>
+  </si>
+  <si>
+    <t>página dos administradores</t>
+  </si>
+  <si>
+    <t>conexão entre site, api e o banco de dados</t>
+  </si>
+  <si>
+    <t>Página acessada apenas por administradores onde poderão publicar noticias aos usuários e analisar a média das avaliações dos usuários e suas opiniões</t>
+  </si>
+  <si>
+    <t>comentário no fórum</t>
+  </si>
+  <si>
+    <t>Funcionalidade de responder postagens no fórum diretamente ao seu autor</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importante </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,6 +221,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +542,7 @@
   <dimension ref="B3:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,23 +555,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="I3" s="5"/>
     </row>
@@ -562,19 +578,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1">
         <v>8</v>
       </c>
       <c r="H4" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -583,19 +599,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
       </c>
       <c r="H5" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -605,19 +621,19 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1">
         <v>8</v>
       </c>
       <c r="H6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="3"/>
@@ -629,19 +645,19 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1">
         <v>13</v>
       </c>
       <c r="H7" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="3"/>
@@ -652,19 +668,19 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
         <v>13</v>
       </c>
       <c r="H8" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -673,19 +689,19 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G9" s="1">
         <v>5</v>
       </c>
       <c r="H9" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -694,44 +710,45 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G10" s="1">
         <v>13</v>
       </c>
       <c r="H10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="1">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="3"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -739,42 +756,66 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G12" s="1">
         <v>21</v>
       </c>
       <c r="H12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1">
+        <v>9</v>
+      </c>
+      <c r="I13" s="10"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1">
+        <v>21</v>
+      </c>
+      <c r="H14" s="1">
+        <v>11</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="3"/>
     </row>
@@ -895,5 +936,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>